<commit_message>
resolução de exercícios sobre o menor caminho
</commit_message>
<xml_diff>
--- a/PesquisaOperacional/3/0722/problemaMenorCaminho.xlsx
+++ b/PesquisaOperacional/3/0722/problemaMenorCaminho.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADM\Downloads\Nova pasta\faculdade2019\PesquisaOperacional\3\0722\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
@@ -205,13 +205,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -497,7 +497,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G2" sqref="G2:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,15 +538,15 @@
       <c r="C2" s="2">
         <v>40</v>
       </c>
-      <c r="D2" s="8">
-        <v>0</v>
+      <c r="D2" s="6">
+        <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="2">
-        <f ca="1">SUMIF($B$2:$B$8,G2,$D$2:$D$8)-SUMIF($A$2:$A$8,G2,$D$2:$D$8)</f>
-        <v>0</v>
+        <f>SUMIF($B$2:$B$8,F2,$D$2:$D$8)-SUMIF($A$2:$A$8,F2,$D$2:$D$8)</f>
+        <v>-1</v>
       </c>
       <c r="H2" s="2">
         <v>-1</v>
@@ -562,14 +562,14 @@
       <c r="C3" s="2">
         <v>30</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="6">
         <v>0</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G7" ca="1" si="0">SUMIF($B$2:$B$8,G3,$D$2:$D$8)-SUMIF($A$2:$A$8,G3,$D$2:$D$8)</f>
+        <f t="shared" ref="G3:G7" si="0">SUMIF($B$2:$B$8,F3,$D$2:$D$8)-SUMIF($A$2:$A$8,F3,$D$2:$D$8)</f>
         <v>0</v>
       </c>
       <c r="H3" s="2">
@@ -586,14 +586,14 @@
       <c r="C4" s="2">
         <v>30</v>
       </c>
-      <c r="D4" s="8">
-        <v>0</v>
+      <c r="D4" s="6">
+        <v>1</v>
       </c>
       <c r="F4" s="2">
         <v>2</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4" s="2">
@@ -610,14 +610,14 @@
       <c r="C5" s="2">
         <v>20</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="6">
         <v>0</v>
       </c>
       <c r="F5" s="2">
         <v>3</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H5" s="2">
@@ -634,14 +634,14 @@
       <c r="C6" s="2">
         <v>30</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <v>0</v>
       </c>
       <c r="F6" s="2">
         <v>4</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H6" s="2">
@@ -658,15 +658,15 @@
       <c r="C7" s="2">
         <v>20</v>
       </c>
-      <c r="D7" s="8">
-        <v>0</v>
+      <c r="D7" s="6">
+        <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="H7" s="2">
         <v>1</v>
@@ -682,7 +682,7 @@
       <c r="C8" s="2">
         <v>20</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="6">
         <v>0</v>
       </c>
       <c r="E8" s="1"/>
@@ -702,13 +702,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="8"/>
       <c r="D10" s="3">
         <f>SUMPRODUCT(C2:C8,D2:D8)</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>

</xml_diff>